<commit_message>
i18n of questionnaire static strings
</commit_message>
<xml_diff>
--- a/molgenis-core-ui/src/main/resources/i18n.xlsx
+++ b/molgenis-core-ui/src/main/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="1220" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16500" yWindow="4540" windowWidth="13700" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i18nstrings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>msgid</t>
   </si>
@@ -113,13 +113,106 @@
   </si>
   <si>
     <t>Wizard</t>
+  </si>
+  <si>
+    <t>questionnaires_title</t>
+  </si>
+  <si>
+    <t>My questionnaires</t>
+  </si>
+  <si>
+    <t>questionnaires_description</t>
+  </si>
+  <si>
+    <t>Submitted and open questionnaires</t>
+  </si>
+  <si>
+    <t>questionnaires_table_questionnaire_header</t>
+  </si>
+  <si>
+    <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>questionnaires_table_status_header</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>questionnaires_table_view_questionnaire_button</t>
+  </si>
+  <si>
+    <t>View questionnaire</t>
+  </si>
+  <si>
+    <t>questionnaires_table_start_questionnaire_button</t>
+  </si>
+  <si>
+    <t>questionnaires_table_continue_questionnaire_button</t>
+  </si>
+  <si>
+    <t>Start questionnaire</t>
+  </si>
+  <si>
+    <t>Continue questionnaire</t>
+  </si>
+  <si>
+    <t>questionnaires_no_questionnaires_found_message</t>
+  </si>
+  <si>
+    <t>No questionnaires found</t>
+  </si>
+  <si>
+    <t>questionnaires_table_status_not_started</t>
+  </si>
+  <si>
+    <t>Not started yet</t>
+  </si>
+  <si>
+    <t>questionnaires_table_status_open</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>questionnaires_table_status_submitted</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>questionnaire_back_button</t>
+  </si>
+  <si>
+    <t>Back to my questionnaires</t>
+  </si>
+  <si>
+    <t>form_bool_true</t>
+  </si>
+  <si>
+    <t>form_bool_false</t>
+  </si>
+  <si>
+    <t>form_bool_missing</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>questionnaire_thank_you_page_back_button</t>
+  </si>
+  <si>
+    <t>Back to My questionnaires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +223,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,14 +261,67 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,16 +651,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -510,111 +672,240 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -627,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove languages from i18n.xlsx Disable meta data editing for some entitity/attribute meta data attributes Increase number of allowed attribute meta data edit type updates Improve PostgreSQL exception translation for type updates
</commit_message>
<xml_diff>
--- a/molgenis-core-ui/src/main/resources/i18n.xlsx
+++ b/molgenis-core-ui/src/main/resources/i18n.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="2660" windowWidth="13700" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="1875" yWindow="2655" windowWidth="13695" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i18nstrings" sheetId="1" r:id="rId1"/>
-    <sheet name="languages" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>msgid</t>
   </si>
@@ -62,15 +61,6 @@
   </si>
   <si>
     <t>No results found</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>English</t>
   </si>
   <si>
     <t>questionnaire_save_and_continue</t>
@@ -416,6 +406,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -743,17 +738,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="42.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,292 +756,292 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1058,40 +1053,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring and tests for #5120 (#5150)
* Remove deprecated FIXME

* Remove unused attribute storage in MetaDataChanges

* Update javadoc

* Add deleteAll(Strean<Object> ids)

* Remove unused methods

* FIX deleteAll calls wrong method on delegate

* FIX tags can belong to multiple entities. so do not delete tags when deleting entity

* Refactor updateEntityMetaData, add tests

* Split MetaDataService.addEntityMetaData in addEntityMetaData and createRepository

* ENH meta data service tests

* Remove languages from i18n.xlsx
Disable meta data editing for some entitity/attribute meta data attributes
Increase number of allowed attribute meta data edit type updates
Improve PostgreSQL exception translation for type updates

* Replace fully qualified name with import + name
</commit_message>
<xml_diff>
--- a/molgenis-core-ui/src/main/resources/i18n.xlsx
+++ b/molgenis-core-ui/src/main/resources/i18n.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="2660" windowWidth="13700" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="1875" yWindow="2655" windowWidth="13695" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i18nstrings" sheetId="1" r:id="rId1"/>
-    <sheet name="languages" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>msgid</t>
   </si>
@@ -62,15 +61,6 @@
   </si>
   <si>
     <t>No results found</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>English</t>
   </si>
   <si>
     <t>questionnaire_save_and_continue</t>
@@ -416,6 +406,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -743,17 +738,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="42.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,292 +756,292 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1058,40 +1053,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>